<commit_message>
CPP and QPP update
Updated for 2020 and 2021 Rate for contribution only
</commit_message>
<xml_diff>
--- a/srpp/params/cpp_history.xlsx
+++ b/srpp/params/cpp_history.xlsx
@@ -1,32 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UQAM/git/cpp/params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\srpp\srpp\params\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975BB47D-1041-4CE0-90C1-AA0A2B218DE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46120" windowHeight="25300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cppyear" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -155,12 +159,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -298,6 +302,12 @@
     <font>
       <sz val="12"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -650,7 +660,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -667,6 +677,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1021,27 +1034,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO6" sqref="AO6"/>
+      <selection pane="bottomRight" activeCell="F55" sqref="F55:F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="13" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="28" width="10.83203125" style="1"/>
-    <col min="31" max="31" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="10.83203125" style="13"/>
+    <col min="2" max="11" width="10.875" style="1"/>
+    <col min="12" max="13" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="28" width="10.875" style="1"/>
+    <col min="31" max="31" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1173,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1966</v>
       </c>
@@ -1279,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1967</v>
       </c>
@@ -1398,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1968</v>
       </c>
@@ -1517,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1969</v>
       </c>
@@ -1636,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1970</v>
       </c>
@@ -1755,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1971</v>
       </c>
@@ -1874,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1972</v>
       </c>
@@ -1993,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1973</v>
       </c>
@@ -2112,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1974</v>
       </c>
@@ -2231,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1975</v>
       </c>
@@ -2350,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1976</v>
       </c>
@@ -2469,7 +2482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1977</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1978</v>
       </c>
@@ -2707,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1979</v>
       </c>
@@ -2826,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1980</v>
       </c>
@@ -2945,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1981</v>
       </c>
@@ -3064,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1982</v>
       </c>
@@ -3183,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1983</v>
       </c>
@@ -3302,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1984</v>
       </c>
@@ -3421,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1985</v>
       </c>
@@ -3540,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1986</v>
       </c>
@@ -3659,7 +3672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1987</v>
       </c>
@@ -3778,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1988</v>
       </c>
@@ -3897,7 +3910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1989</v>
       </c>
@@ -4016,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1990</v>
       </c>
@@ -4135,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1991</v>
       </c>
@@ -4254,7 +4267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1992</v>
       </c>
@@ -4373,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1993</v>
       </c>
@@ -4492,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1994</v>
       </c>
@@ -4611,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1995</v>
       </c>
@@ -4730,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1996</v>
       </c>
@@ -4849,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1997</v>
       </c>
@@ -4968,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1998</v>
       </c>
@@ -5087,7 +5100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1999</v>
       </c>
@@ -5206,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2000</v>
       </c>
@@ -5325,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2001</v>
       </c>
@@ -5444,7 +5457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2002</v>
       </c>
@@ -5563,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2003</v>
       </c>
@@ -5682,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2004</v>
       </c>
@@ -5801,7 +5814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2005</v>
       </c>
@@ -5920,7 +5933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2006</v>
       </c>
@@ -6039,7 +6052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2007</v>
       </c>
@@ -6158,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2008</v>
       </c>
@@ -6277,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2009</v>
       </c>
@@ -6396,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2010</v>
       </c>
@@ -6515,7 +6528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2011</v>
       </c>
@@ -6634,7 +6647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2012</v>
       </c>
@@ -6753,7 +6766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2013</v>
       </c>
@@ -6872,7 +6885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2014</v>
       </c>
@@ -6991,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2015</v>
       </c>
@@ -7110,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2016</v>
       </c>
@@ -7229,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2017</v>
       </c>
@@ -7348,7 +7361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2018</v>
       </c>
@@ -7467,24 +7480,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2019</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="16">
         <v>57400</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="16">
         <v>3500</v>
       </c>
-      <c r="D55" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="E55" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="F55" s="5">
-        <v>9.9000000000000005E-2</v>
+      <c r="D55" s="17">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E55" s="17">
+        <f>D55</f>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F55" s="18">
+        <v>0.10199999999999999</v>
       </c>
       <c r="G55" s="5">
         <v>7.1999999999999995E-2</v>
@@ -7581,25 +7595,25 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>2020</v>
       </c>
-      <c r="B56" s="3">
-        <f>B55*1.03</f>
-        <v>59122</v>
-      </c>
-      <c r="C56" s="3">
+      <c r="B56" s="16">
+        <v>58700</v>
+      </c>
+      <c r="C56" s="16">
         <v>3500</v>
       </c>
-      <c r="D56" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="F56" s="5">
-        <v>9.9000000000000005E-2</v>
+      <c r="D56" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="E56" s="17">
+        <f t="shared" ref="E56:E57" si="0">D56</f>
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F56" s="18">
+        <v>0.105</v>
       </c>
       <c r="G56" s="5">
         <v>7.1999999999999995E-2</v>
@@ -7700,25 +7714,25 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>2021</v>
       </c>
-      <c r="B57" s="3">
-        <f t="shared" ref="B57:B61" si="0">B56*1.03</f>
-        <v>60895.66</v>
-      </c>
-      <c r="C57" s="3">
+      <c r="B57" s="16">
+        <v>61600</v>
+      </c>
+      <c r="C57" s="16">
         <v>3500</v>
       </c>
-      <c r="D57" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="E57" s="4">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="F57" s="5">
-        <v>9.9000000000000005E-2</v>
+      <c r="D57" s="17">
+        <v>5.45E-2</v>
+      </c>
+      <c r="E57" s="17">
+        <f t="shared" si="0"/>
+        <v>5.45E-2</v>
+      </c>
+      <c r="F57" s="18">
+        <v>0.109</v>
       </c>
       <c r="G57" s="5">
         <v>7.1999999999999995E-2</v>
@@ -7819,13 +7833,13 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>2022</v>
       </c>
       <c r="B58" s="3">
-        <f t="shared" si="0"/>
-        <v>62722.529800000004</v>
+        <f t="shared" ref="B57:B61" si="3">B57*1.03</f>
+        <v>63448</v>
       </c>
       <c r="C58" s="3">
         <v>3500</v>
@@ -7938,13 +7952,13 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>2023</v>
       </c>
       <c r="B59" s="3">
-        <f t="shared" si="0"/>
-        <v>64604.205694000004</v>
+        <f t="shared" si="3"/>
+        <v>65351.44</v>
       </c>
       <c r="C59" s="3">
         <v>3500</v>
@@ -8057,13 +8071,13 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>2024</v>
       </c>
       <c r="B60" s="3">
-        <f t="shared" si="0"/>
-        <v>66542.331864820007</v>
+        <f t="shared" si="3"/>
+        <v>67311.983200000002</v>
       </c>
       <c r="C60" s="3">
         <v>3500</v>
@@ -8176,13 +8190,13 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>2025</v>
       </c>
       <c r="B61" s="3">
-        <f t="shared" si="0"/>
-        <v>68538.601820764612</v>
+        <f t="shared" si="3"/>
+        <v>69331.342696000007</v>
       </c>
       <c r="C61" s="3">
         <v>3500</v>

</xml_diff>